<commit_message>
added some initial vf implementation
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/CondensationSequence/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/PycharmProjects/CondensationSequence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE6C07DF-75E4-FB4B-9304-9F1AC9C3B371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B3ECC6-F7FB-5848-830A-1081FFA1E152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="500" windowWidth="17960" windowHeight="15960" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="11820" yWindow="500" windowWidth="29400" windowHeight="21280" activeTab="2" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
   <si>
     <t>R1</t>
   </si>
@@ -347,42 +347,6 @@
     <t>K2</t>
   </si>
   <si>
-    <t>Th</t>
-  </si>
-  <si>
-    <t>ThO</t>
-  </si>
-  <si>
-    <t>ThO2</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>UO</t>
-  </si>
-  <si>
-    <t>UO2</t>
-  </si>
-  <si>
-    <t>UO3</t>
-  </si>
-  <si>
-    <t>Pu</t>
-  </si>
-  <si>
-    <t>PuO</t>
-  </si>
-  <si>
-    <t>PuO2</t>
-  </si>
-  <si>
-    <t>O2</t>
-  </si>
-  <si>
-    <t>R37</t>
-  </si>
-  <si>
     <t>O2_g</t>
   </si>
   <si>
@@ -425,30 +389,6 @@
     <t>Product 2</t>
   </si>
   <si>
-    <t>Si_g</t>
-  </si>
-  <si>
-    <t>O_g</t>
-  </si>
-  <si>
-    <t>Fe_g</t>
-  </si>
-  <si>
-    <t>Al_g</t>
-  </si>
-  <si>
-    <t>Ti_g</t>
-  </si>
-  <si>
-    <t>Th_g</t>
-  </si>
-  <si>
-    <t>U_g</t>
-  </si>
-  <si>
-    <t>Pu_g</t>
-  </si>
-  <si>
     <t>Stoich Product 1</t>
   </si>
   <si>
@@ -456,39 +396,6 @@
   </si>
   <si>
     <t>Reactant</t>
-  </si>
-  <si>
-    <t>SiO2_liq</t>
-  </si>
-  <si>
-    <t>MgO_liq</t>
-  </si>
-  <si>
-    <t>FeO_liq</t>
-  </si>
-  <si>
-    <t>CaO_liq</t>
-  </si>
-  <si>
-    <t>Al2O3_Liq</t>
-  </si>
-  <si>
-    <t>TiO2_liq</t>
-  </si>
-  <si>
-    <t>Na2O_liq</t>
-  </si>
-  <si>
-    <t>K2O_liq</t>
-  </si>
-  <si>
-    <t>ThO2_liq</t>
-  </si>
-  <si>
-    <t>UO2_liq</t>
-  </si>
-  <si>
-    <t>PuO2_liq</t>
   </si>
 </sst>
 </file>
@@ -846,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA51B45C-F7CC-3B41-AC8C-EF614A95CDBA}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,19 +766,19 @@
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
         <v>37</v>
@@ -885,10 +792,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -897,7 +804,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="G2">
         <v>22.13</v>
@@ -911,10 +818,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -923,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="G3">
         <v>12.56</v>
@@ -937,10 +844,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -949,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="G4">
         <v>12.06</v>
@@ -963,10 +870,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -975,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="G5">
         <v>11.88</v>
@@ -989,10 +896,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1001,7 +908,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="G6">
         <v>35.83</v>
@@ -1015,10 +922,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1027,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="G7">
         <v>21.07</v>
@@ -1041,10 +948,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1053,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="G8">
         <v>15.56</v>
@@ -1067,10 +974,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1079,91 +986,13 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="G9">
         <v>15.33</v>
       </c>
       <c r="H9">
         <v>-36735</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>148</v>
-      </c>
-      <c r="G10">
-        <v>20.43</v>
-      </c>
-      <c r="H10">
-        <v>-112807</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>149</v>
-      </c>
-      <c r="G11">
-        <v>19.18</v>
-      </c>
-      <c r="H11">
-        <v>-100627</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G12">
-        <v>18.670000000000002</v>
-      </c>
-      <c r="H12">
-        <v>-91886</v>
       </c>
     </row>
   </sheetData>
@@ -1174,11 +1003,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB38BCC-BF73-D341-9EF2-69884C8E8DA9}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A7"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,40 +1026,40 @@
         <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="H1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="I1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="J1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="K1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="L1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="M1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="N1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="O1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="P1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1515,7 +1344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1532,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1552,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1572,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1589,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1609,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1626,7 +1455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1646,7 +1475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1663,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1683,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1700,7 +1529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1718,214 +1547,6 @@
       </c>
       <c r="M27">
         <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28">
-        <v>5.96</v>
-      </c>
-      <c r="D28">
-        <v>-29600</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29">
-        <v>2.75</v>
-      </c>
-      <c r="D29">
-        <v>3497</v>
-      </c>
-      <c r="E29">
-        <v>0.5</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30">
-        <v>-1.58</v>
-      </c>
-      <c r="D30">
-        <v>28875</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="N30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31">
-        <v>5.75</v>
-      </c>
-      <c r="D31">
-        <v>-25470</v>
-      </c>
-      <c r="O31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32">
-        <v>3.02</v>
-      </c>
-      <c r="D32">
-        <v>1705</v>
-      </c>
-      <c r="E32">
-        <v>0.5</v>
-      </c>
-      <c r="O32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33">
-        <v>-1.19</v>
-      </c>
-      <c r="D33">
-        <v>26554</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="O33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34">
-        <v>-4.24</v>
-      </c>
-      <c r="D34">
-        <v>43710</v>
-      </c>
-      <c r="E34">
-        <v>1.5</v>
-      </c>
-      <c r="O34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35">
-        <v>4.79</v>
-      </c>
-      <c r="D35">
-        <v>-17316</v>
-      </c>
-      <c r="E35">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36">
-        <v>2.4</v>
-      </c>
-      <c r="D36">
-        <v>6875</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="P36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37">
-        <v>-1.76</v>
-      </c>
-      <c r="D37">
-        <v>25984</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="P37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1938,9 +1559,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575B768E-B263-7849-9255-8DC0D8CFF25A}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2742,5 +2363,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>